<commit_message>
exell grafik blitzeblank schön super duper
</commit_message>
<xml_diff>
--- a/Datenstrukturen und Algorithmen/Übungsserie 6/Auswertung.xlsx
+++ b/Datenstrukturen und Algorithmen/Übungsserie 6/Auswertung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alana\myCloud\UNIBE\Informatik\Datenstrukturen und Algorithmen\Git_mit_Sandro\Unistuff\Datenstrukturen und Algorithmen\Übungsserie 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1F4C18-D2E2-4CB9-AEC4-376B0DE623A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F1DF87-42F8-4B12-A7DF-583B8D2980B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="27977" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -559,6 +559,7 @@
         <c:axId val="773549632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="2500"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -671,11 +672,13 @@
         <c:crossAx val="773542976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="250"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="773542976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="9"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1735,7 +1738,7 @@
   <dimension ref="A2:AE1631"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E102" zoomScale="154" workbookViewId="0">
-      <selection activeCell="R110" sqref="R110"/>
+      <selection activeCell="Q118" sqref="Q118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>